<commit_message>
Fixed CORS, cleaned up duplicate app definition, set production port
</commit_message>
<xml_diff>
--- a/checkins.xlsx
+++ b/checkins.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -514,9 +514,55 @@
         <v>Brian Gichobi</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>9fe83a0f-e574-4337-9aa4-fa11e0a8075d</v>
+      </c>
+      <c r="B6">
+        <v>-1.293631102816713</v>
+      </c>
+      <c r="C6">
+        <v>36.80742457755191</v>
+      </c>
+      <c r="D6" t="str">
+        <v>2025-10-28</v>
+      </c>
+      <c r="E6" t="str">
+        <v>10:26:28 AM</v>
+      </c>
+      <c r="F6" t="str">
+        <v>::1</v>
+      </c>
+      <c r="G6" t="str">
+        <v>test</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>01735368-36c0-43b2-a7f8-3af44c2a1dff</v>
+      </c>
+      <c r="B7">
+        <v>-1.2936585497144812</v>
+      </c>
+      <c r="C7">
+        <v>36.80746346087199</v>
+      </c>
+      <c r="D7" t="str">
+        <v>2025-10-28</v>
+      </c>
+      <c r="E7" t="str">
+        <v>10:34:00 AM</v>
+      </c>
+      <c r="F7" t="str">
+        <v>::1</v>
+      </c>
+      <c r="G7" t="str">
+        <v>brian</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G7"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>